<commit_message>
all submodules are successfully chained together, achieving end2end data processing
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421FE7F4-1E3B-F843-B51E-95221D1EFB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78330141-4A2F-D546-8DA4-9718C21D797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5960" windowWidth="34200" windowHeight="13040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -36,43 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
-  <si>
-    <t>A2LName</t>
-  </si>
-  <si>
-    <t>TactName</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>VehicleSpeed</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>LMCAutoBrkEnabled</t>
-  </si>
-  <si>
-    <t>DADCAxLmtIT4</t>
-  </si>
-  <si>
-    <t>FLWheelBrakeTorqueEst2</t>
-  </si>
-  <si>
-    <t>FRWheelBrakeTorqueEst2</t>
-  </si>
-  <si>
-    <t>RLWheelBrakeTorqueEst2</t>
-  </si>
-  <si>
-    <t>RRWheelBrakeTorqueEst2</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -83,66 +47,30 @@
     <t>acceleration[1]</t>
   </si>
   <si>
-    <t>brake_torque_wheels[0]</t>
-  </si>
-  <si>
-    <t>brake_torque_wheels[1]</t>
-  </si>
-  <si>
-    <t>brake_torque_wheels[2]</t>
-  </si>
-  <si>
-    <t>brake_torque_wheels[3]</t>
-  </si>
-  <si>
-    <t>aeb_request</t>
-  </si>
-  <si>
-    <t>Raster</t>
-  </si>
-  <si>
     <t>imuFrame</t>
   </si>
   <si>
     <t>vehicleIOASILCommandE2EWrapper</t>
   </si>
   <si>
-    <t>aebRequest</t>
-  </si>
-  <si>
-    <t>vehicleIOQMState</t>
-  </si>
-  <si>
     <t>vehicleIOstate</t>
   </si>
   <si>
     <t>throttle_value</t>
   </si>
   <si>
-    <t>PedalPosPro</t>
-  </si>
-  <si>
     <t>active_safety_settings/AEB/abort_any_active_events</t>
   </si>
   <si>
-    <t>VCSAbort</t>
-  </si>
-  <si>
     <t>DICommand</t>
   </si>
   <si>
     <t>brake_pedal_pressed</t>
   </si>
   <si>
-    <t>BrakePedalPressed</t>
-  </si>
-  <si>
     <t>steering_wheel_angle</t>
   </si>
   <si>
-    <t>SteerAngle</t>
-  </si>
-  <si>
     <t>Output_name</t>
   </si>
   <si>
@@ -212,9 +140,6 @@
     <t>LateralAcceleration_th</t>
   </si>
   <si>
-    <t>Long_Clearance</t>
-  </si>
-  <si>
     <t>Long_Clearance [m]</t>
   </si>
   <si>
@@ -239,15 +164,9 @@
     <t>steering_wheel_angle_speed</t>
   </si>
   <si>
-    <t>SteerAngle_Rate</t>
-  </si>
-  <si>
     <t>turnrate[2]</t>
   </si>
   <si>
-    <t>YawRate</t>
-  </si>
-  <si>
     <t>aeb_state_info/aeb_full_state_info/longitudinal_clearance</t>
   </si>
   <si>
@@ -287,9 +206,6 @@
     <t>isVehStopped</t>
   </si>
   <si>
-    <t>isPedalOnAtStrt</t>
-  </si>
-  <si>
     <t>Ego Speed</t>
   </si>
   <si>
@@ -336,13 +252,82 @@
   </si>
   <si>
     <t>Longitudinal Clearance [m]</t>
+  </si>
+  <si>
+    <t>channelGroup</t>
+  </si>
+  <si>
+    <t>synonym</t>
+  </si>
+  <si>
+    <t>genericName</t>
+  </si>
+  <si>
+    <t>raster</t>
+  </si>
+  <si>
+    <t>latActAccel</t>
+  </si>
+  <si>
+    <t>longActAccel</t>
+  </si>
+  <si>
+    <t>aebTargetDecel</t>
+  </si>
+  <si>
+    <t>speedESC</t>
+  </si>
+  <si>
+    <t>egoSpeed</t>
+  </si>
+  <si>
+    <t>throttleValue</t>
+  </si>
+  <si>
+    <t>aebAbortFromVcs</t>
+  </si>
+  <si>
+    <t>brakePedalPressed</t>
+  </si>
+  <si>
+    <t>steerWheelAngle</t>
+  </si>
+  <si>
+    <t>steerWheelAngleSpeed</t>
+  </si>
+  <si>
+    <t>yawRate</t>
+  </si>
+  <si>
+    <t>aeb_state_info/most_relevant_object_id</t>
+  </si>
+  <si>
+    <t>targetId</t>
+  </si>
+  <si>
+    <t>aeb_state_info/time_to_collision</t>
+  </si>
+  <si>
+    <t>ttc</t>
+  </si>
+  <si>
+    <t>aeb_state_info/aeb_full_state_info/state</t>
+  </si>
+  <si>
+    <t>aebFullState</t>
+  </si>
+  <si>
+    <t>aeb_state_info/aeb_partial_state_info/state</t>
+  </si>
+  <si>
+    <t>aebPartialState</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +355,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -407,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,6 +424,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,215 +740,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="C4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>28</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>71</v>
+      <c r="B14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>19</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +990,7 @@
   <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,39 +1007,39 @@
   <sheetData>
     <row r="2" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -1021,27 +1048,27 @@
         <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1050,27 +1077,27 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1079,27 +1106,27 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1108,27 +1135,27 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1137,27 +1164,27 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1166,27 +1193,27 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1195,27 +1222,27 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1224,27 +1251,27 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1253,19 +1280,19 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1285,13 +1312,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove the condTrue in the csv and optimze plotEnabled logic
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78330141-4A2F-D546-8DA4-9718C21D797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C1A11-AA1E-8749-8A84-65BE0C080079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="5620" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Axis_Name</t>
   </si>
   <si>
-    <t>Condition_Var</t>
-  </si>
-  <si>
     <t>Calibration_Lim</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>aebStateInfo</t>
   </si>
   <si>
-    <t>condTrue</t>
-  </si>
-  <si>
     <t>vehSpd</t>
   </si>
   <si>
@@ -321,6 +315,9 @@
   </si>
   <si>
     <t>aebPartialState</t>
+  </si>
+  <si>
+    <t>plotEnabled</t>
   </si>
 </sst>
 </file>
@@ -756,16 +753,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>3</v>
@@ -790,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>3</v>
@@ -804,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>4</v>
@@ -815,10 +812,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>5</v>
@@ -832,7 +829,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>5</v>
@@ -846,7 +843,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>8</v>
@@ -860,7 +857,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>5</v>
@@ -874,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>5</v>
@@ -885,10 +882,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>5</v>
@@ -899,10 +896,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>3</v>
@@ -913,13 +910,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -927,13 +924,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -941,13 +938,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -955,13 +952,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -969,13 +966,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +987,7 @@
   <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1022,24 +1019,24 @@
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -1048,27 +1045,27 @@
         <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1077,27 +1074,27 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1106,27 +1103,27 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1135,27 +1132,27 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1164,27 +1161,27 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1193,27 +1190,27 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1222,27 +1219,27 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1251,27 +1248,27 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1280,19 +1277,19 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1312,13 +1309,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
visScatterPlotter optimized when plotEnabled is false
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C1A11-AA1E-8749-8A84-65BE0C080079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260E95A-0B65-524A-B46A-871A3DC56ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="5620" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5620" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
modify the visScatterPlotter to update the x-axis based on data from the excel file
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260E95A-0B65-524A-B46A-871A3DC56ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02DFA47-C32D-BB4B-BD77-12AE95E9A1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5620" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5060" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -92,54 +92,27 @@
     <t>Legend</t>
   </si>
   <si>
-    <t>Veh_Spd</t>
-  </si>
-  <si>
-    <t>Vehicle Speed [kph]</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>Time [sec]</t>
-  </si>
-  <si>
-    <t>PedalPos [%]</t>
-  </si>
-  <si>
     <t>PedalPosProIncrease_Th</t>
   </si>
   <si>
-    <t>Steering_Angle [rad]</t>
-  </si>
-  <si>
     <t>SteeringWheelAngle_Th</t>
   </si>
   <si>
-    <t>Steering_Angle_Rate [rad/s]</t>
-  </si>
-  <si>
     <t>AEB_SteeringAngleRate_Override</t>
   </si>
   <si>
-    <t>Yaw_Rate [rad/s]</t>
-  </si>
-  <si>
     <t>YawrateSuspension_Th</t>
   </si>
   <si>
-    <t>Lat_Acceleration [m/s2]</t>
-  </si>
-  <si>
     <t>LateralAcceleration_th</t>
   </si>
   <si>
-    <t>Long_Clearance [m]</t>
-  </si>
-  <si>
     <t>Longitudinal Clearance</t>
   </si>
   <si>
@@ -242,9 +215,6 @@
     <t>Max Yaw Rate [rad/s]</t>
   </si>
   <si>
-    <t>Max Lateral Acceleration [[m/s2]</t>
-  </si>
-  <si>
     <t>Longitudinal Clearance [m]</t>
   </si>
   <si>
@@ -318,6 +288,30 @@
   </si>
   <si>
     <t>plotEnabled</t>
+  </si>
+  <si>
+    <t>Max Lateral Acceleration [m/s2]</t>
+  </si>
+  <si>
+    <t>Ego Speed (km/h)</t>
+  </si>
+  <si>
+    <t>Time (sec)</t>
+  </si>
+  <si>
+    <t>Percentage (%)</t>
+  </si>
+  <si>
+    <t>Angle (rad)</t>
+  </si>
+  <si>
+    <t>Angle Speed (rad/s)</t>
+  </si>
+  <si>
+    <t>Acceleration (m/s2)</t>
+  </si>
+  <si>
+    <t>Distance (m)</t>
   </si>
 </sst>
 </file>
@@ -753,16 +747,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -773,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>3</v>
@@ -787,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>3</v>
@@ -801,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>4</v>
@@ -812,10 +806,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>5</v>
@@ -829,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>5</v>
@@ -843,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>8</v>
@@ -857,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>5</v>
@@ -871,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>5</v>
@@ -882,10 +876,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>5</v>
@@ -896,10 +890,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>3</v>
@@ -910,13 +904,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -924,13 +918,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -938,13 +932,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -952,13 +946,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -966,13 +960,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -986,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1013,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>16</v>
@@ -1028,44 +1022,44 @@
         <v>17</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>150</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1074,27 +1068,27 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1103,27 +1097,27 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1132,27 +1126,27 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1161,27 +1155,27 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1190,27 +1184,27 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1219,27 +1213,27 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1248,27 +1242,27 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1277,19 +1271,19 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1309,13 +1303,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
group graphs of the same title into one figure
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02DFA47-C32D-BB4B-BD77-12AE95E9A1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEFF1FF-C05E-B14C-A556-1DC9592FD2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5060" windowWidth="34200" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="7480" windowWidth="34200" windowHeight="13600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
     <sheet name="graphSpec" sheetId="3" r:id="rId2"/>
-    <sheet name="lineColors" sheetId="4" r:id="rId3"/>
+    <sheet name="markerShapes" sheetId="5" r:id="rId3"/>
+    <sheet name="lineColors" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -71,9 +72,6 @@
     <t>steering_wheel_angle</t>
   </si>
   <si>
-    <t>Output_name</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -113,18 +111,6 @@
     <t>LateralAcceleration_th</t>
   </si>
   <si>
-    <t>Longitudinal Clearance</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>plotType</t>
   </si>
   <si>
@@ -197,27 +183,6 @@
     <t>Max Lateral Acceleration</t>
   </si>
   <si>
-    <t>Dead Time [s]</t>
-  </si>
-  <si>
-    <t>Intervention Duration [s]</t>
-  </si>
-  <si>
-    <t>Max Throttle Value [%]</t>
-  </si>
-  <si>
-    <t>Max Steering Angle [%]</t>
-  </si>
-  <si>
-    <t>Max Steering Rate [%]</t>
-  </si>
-  <si>
-    <t>Max Yaw Rate [rad/s]</t>
-  </si>
-  <si>
-    <t>Longitudinal Clearance [m]</t>
-  </si>
-  <si>
     <t>channelGroup</t>
   </si>
   <si>
@@ -290,9 +255,6 @@
     <t>plotEnabled</t>
   </si>
   <si>
-    <t>Max Lateral Acceleration [m/s2]</t>
-  </si>
-  <si>
     <t>Ego Speed (km/h)</t>
   </si>
   <si>
@@ -312,6 +274,75 @@
   </si>
   <si>
     <t>Distance (m)</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Stable Detection Dist</t>
+  </si>
+  <si>
+    <t>AEB Actuation Dist</t>
+  </si>
+  <si>
+    <t>AEB Stop Gap</t>
+  </si>
+  <si>
+    <t>stableDetDist</t>
+  </si>
+  <si>
+    <t>aebIntvDist</t>
+  </si>
+  <si>
+    <t>aebStopGap</t>
+  </si>
+  <si>
+    <t>AEB Braking Distances</t>
+  </si>
+  <si>
+    <t>ConnectPoints</t>
+  </si>
+  <si>
+    <t>firstDetDist</t>
+  </si>
+  <si>
+    <t>First Detection Dist</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Shapes</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -396,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,17 +437,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,227 +774,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D10" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="D13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
-        <v>14</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="D14" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>14</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="D15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>28</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>15</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>14</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>15</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>2</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>19</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>19</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
-        <v>19</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>34</v>
+      <c r="D16" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -978,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -994,43 +1022,47 @@
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -1039,27 +1071,30 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1068,27 +1103,30 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1097,27 +1135,30 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1126,27 +1167,30 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1155,27 +1199,30 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1184,27 +1231,30 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1213,27 +1263,30 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1242,48 +1295,150 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="K10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11" s="3">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
         <v>5</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>30</v>
+      <c r="K12" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1292,100 +1447,160 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1821CB-8E60-1A45-8122-C329B6E1FCF3}">
+  <dimension ref="B1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1943DE-263B-CE4F-869C-DE791D333F1F}">
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.44700000000000001</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.74099999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.85</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.32500000000000001</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.92900000000000005</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.69399999999999995</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.49399999999999999</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.184</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.55600000000000005</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.46600000000000003</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.67400000000000004</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.188</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.30099999999999999</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.745</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.93300000000000005</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.63500000000000001</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>7.8E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mdf2matConv.py-signal extraction based on group and channel name + visScatterPlotter: resolve the issue: failed to display grid and legends when last row of plotEnabled is false
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEFF1FF-C05E-B14C-A556-1DC9592FD2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0461E-72D0-B044-95FA-9D079E940344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="7480" windowWidth="34200" windowHeight="13600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vbRcSignals" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Max Lateral Acceleration</t>
   </si>
   <si>
-    <t>channelGroup</t>
-  </si>
-  <si>
     <t>synonym</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>vehicleIOActuationFeedback</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,6 +444,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,21 +765,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
@@ -783,219 +788,261 @@
       <c r="C1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>15</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>15</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>19</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1008,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1074,7 @@
   <sheetData>
     <row r="2" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1042,7 +1089,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>15</v>
@@ -1054,7 +1101,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
@@ -1071,7 +1118,7 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
@@ -1103,7 +1150,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
@@ -1135,7 +1182,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>39</v>
@@ -1167,7 +1214,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
@@ -1199,7 +1246,7 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
@@ -1231,7 +1278,7 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
@@ -1263,7 +1310,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
@@ -1295,7 +1342,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
@@ -1315,19 +1362,19 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>1</v>
@@ -1336,7 +1383,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>25</v>
@@ -1347,10 +1394,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1359,7 +1406,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>1</v>
@@ -1368,7 +1415,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>25</v>
@@ -1379,10 +1426,10 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1391,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>1</v>
@@ -1400,7 +1447,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>25</v>
@@ -1411,10 +1458,10 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1423,16 +1470,16 @@
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
+        <v>77</v>
+      </c>
+      <c r="G14" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>25</v>
@@ -1458,47 +1505,47 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1943DE-263B-CE4F-869C-DE791D333F1F}">
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1518,13 +1565,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
clean up the processing notifications
</commit_message>
<xml_diff>
--- a/config/SignalMapPlotSpec.xlsx
+++ b/config/SignalMapPlotSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0461E-72D0-B044-95FA-9D079E940344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418BD6F1-1D91-6449-974D-29AA87EA8B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="106">
   <si>
     <t>payload/long_ctrl_accel_request</t>
   </si>
@@ -45,304 +45,316 @@
     <t>acceleration[0]</t>
   </si>
   <si>
+    <t>imuFrame</t>
+  </si>
+  <si>
+    <t>vehicleIOASILCommandE2EWrapper</t>
+  </si>
+  <si>
+    <t>vehicleIOstate</t>
+  </si>
+  <si>
+    <t>throttle_value</t>
+  </si>
+  <si>
+    <t>active_safety_settings/AEB/abort_any_active_events</t>
+  </si>
+  <si>
+    <t>DICommand</t>
+  </si>
+  <si>
+    <t>brake_pedal_pressed</t>
+  </si>
+  <si>
+    <t>steering_wheel_angle</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Min_Axis_value</t>
+  </si>
+  <si>
+    <t>Max_Axis_value</t>
+  </si>
+  <si>
+    <t>Axis_Name</t>
+  </si>
+  <si>
+    <t>Calibration_Lim</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>PedalPosProIncrease_Th</t>
+  </si>
+  <si>
+    <t>SteeringWheelAngle_Th</t>
+  </si>
+  <si>
+    <t>AEB_SteeringAngleRate_Override</t>
+  </si>
+  <si>
+    <t>YawrateSuspension_Th</t>
+  </si>
+  <si>
+    <t>LateralAcceleration_th</t>
+  </si>
+  <si>
+    <t>plotType</t>
+  </si>
+  <si>
+    <t>scatter</t>
+  </si>
+  <si>
+    <t>steering_wheel_angle_speed</t>
+  </si>
+  <si>
+    <t>turnrate[2]</t>
+  </si>
+  <si>
+    <t>aeb_state_info/aeb_full_state_info/longitudinal_clearance</t>
+  </si>
+  <si>
+    <t>aebStateInfo</t>
+  </si>
+  <si>
+    <t>vehSpd</t>
+  </si>
+  <si>
+    <t>m1DeadTime</t>
+  </si>
+  <si>
+    <t>intvDur</t>
+  </si>
+  <si>
+    <t>pedalMax</t>
+  </si>
+  <si>
+    <t>absSteerMaxDeg</t>
+  </si>
+  <si>
+    <t>absSteerRateMaxDeg</t>
+  </si>
+  <si>
+    <t>absYawRateMaxDeg</t>
+  </si>
+  <si>
+    <t>absLatAccelMax</t>
+  </si>
+  <si>
+    <t>longGap</t>
+  </si>
+  <si>
+    <t>isVehStopped</t>
+  </si>
+  <si>
+    <t>Ego Speed</t>
+  </si>
+  <si>
+    <t>Dead Time</t>
+  </si>
+  <si>
+    <t>Intervention Duration</t>
+  </si>
+  <si>
+    <t>Max Throttle Value</t>
+  </si>
+  <si>
+    <t>Max Steering Angle</t>
+  </si>
+  <si>
+    <t>Max Steering Angle Rate</t>
+  </si>
+  <si>
+    <t>Max Yaw Rate</t>
+  </si>
+  <si>
+    <t>Max Lateral Acceleration</t>
+  </si>
+  <si>
+    <t>synonym</t>
+  </si>
+  <si>
+    <t>genericName</t>
+  </si>
+  <si>
+    <t>raster</t>
+  </si>
+  <si>
+    <t>latActAccel</t>
+  </si>
+  <si>
+    <t>longActAccel</t>
+  </si>
+  <si>
+    <t>aebTargetDecel</t>
+  </si>
+  <si>
+    <t>speedESC</t>
+  </si>
+  <si>
+    <t>egoSpeed</t>
+  </si>
+  <si>
+    <t>throttleValue</t>
+  </si>
+  <si>
+    <t>aebAbortFromVcs</t>
+  </si>
+  <si>
+    <t>brakePedalPressed</t>
+  </si>
+  <si>
+    <t>steerWheelAngle</t>
+  </si>
+  <si>
+    <t>steerWheelAngleSpeed</t>
+  </si>
+  <si>
+    <t>yawRate</t>
+  </si>
+  <si>
+    <t>aeb_state_info/most_relevant_object_id</t>
+  </si>
+  <si>
+    <t>targetId</t>
+  </si>
+  <si>
+    <t>aeb_state_info/time_to_collision</t>
+  </si>
+  <si>
+    <t>ttc</t>
+  </si>
+  <si>
+    <t>aeb_state_info/aeb_full_state_info/state</t>
+  </si>
+  <si>
+    <t>aebFullState</t>
+  </si>
+  <si>
+    <t>aeb_state_info/aeb_partial_state_info/state</t>
+  </si>
+  <si>
+    <t>aebPartialState</t>
+  </si>
+  <si>
+    <t>plotEnabled</t>
+  </si>
+  <si>
+    <t>Ego Speed (km/h)</t>
+  </si>
+  <si>
+    <t>Time (sec)</t>
+  </si>
+  <si>
+    <t>Percentage (%)</t>
+  </si>
+  <si>
+    <t>Acceleration (m/s2)</t>
+  </si>
+  <si>
+    <t>Distance (m)</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Stable Detection Dist</t>
+  </si>
+  <si>
+    <t>AEB Actuation Dist</t>
+  </si>
+  <si>
+    <t>AEB Stop Gap</t>
+  </si>
+  <si>
+    <t>stableDetDist</t>
+  </si>
+  <si>
+    <t>aebIntvDist</t>
+  </si>
+  <si>
+    <t>aebStopGap</t>
+  </si>
+  <si>
+    <t>AEB Braking Distances</t>
+  </si>
+  <si>
+    <t>ConnectPoints</t>
+  </si>
+  <si>
+    <t>firstDetDist</t>
+  </si>
+  <si>
+    <t>First Detection Dist</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Shapes</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>vehicleIOActuationFeedback</t>
+  </si>
+  <si>
+    <t>Angle Speed (deg/s)</t>
+  </si>
+  <si>
+    <t>Angle (deg)</t>
+  </si>
+  <si>
     <t>acceleration[1]</t>
   </si>
   <si>
-    <t>imuFrame</t>
-  </si>
-  <si>
-    <t>vehicleIOASILCommandE2EWrapper</t>
-  </si>
-  <si>
-    <t>vehicleIOstate</t>
-  </si>
-  <si>
-    <t>throttle_value</t>
-  </si>
-  <si>
-    <t>active_safety_settings/AEB/abort_any_active_events</t>
-  </si>
-  <si>
-    <t>DICommand</t>
-  </si>
-  <si>
-    <t>brake_pedal_pressed</t>
-  </si>
-  <si>
-    <t>steering_wheel_angle</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Min_Axis_value</t>
-  </si>
-  <si>
-    <t>Max_Axis_value</t>
-  </si>
-  <si>
-    <t>Axis_Name</t>
-  </si>
-  <si>
-    <t>Calibration_Lim</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>PedalPosProIncrease_Th</t>
-  </si>
-  <si>
-    <t>SteeringWheelAngle_Th</t>
-  </si>
-  <si>
-    <t>AEB_SteeringAngleRate_Override</t>
-  </si>
-  <si>
-    <t>YawrateSuspension_Th</t>
-  </si>
-  <si>
-    <t>LateralAcceleration_th</t>
-  </si>
-  <si>
-    <t>plotType</t>
-  </si>
-  <si>
-    <t>scatter</t>
-  </si>
-  <si>
-    <t>steering_wheel_angle_speed</t>
-  </si>
-  <si>
-    <t>turnrate[2]</t>
-  </si>
-  <si>
-    <t>aeb_state_info/aeb_full_state_info/longitudinal_clearance</t>
-  </si>
-  <si>
-    <t>aebStateInfo</t>
-  </si>
-  <si>
-    <t>vehSpd</t>
-  </si>
-  <si>
-    <t>m1DeadTime</t>
-  </si>
-  <si>
-    <t>intvDur</t>
-  </si>
-  <si>
-    <t>pedalMax</t>
-  </si>
-  <si>
-    <t>absSteerMaxDeg</t>
-  </si>
-  <si>
-    <t>absSteerRateMaxDeg</t>
-  </si>
-  <si>
-    <t>absYawRateMaxDeg</t>
-  </si>
-  <si>
-    <t>absLatAccelMax</t>
-  </si>
-  <si>
-    <t>longGap</t>
-  </si>
-  <si>
-    <t>isVehStopped</t>
-  </si>
-  <si>
-    <t>Ego Speed</t>
-  </si>
-  <si>
-    <t>Dead Time</t>
-  </si>
-  <si>
-    <t>Intervention Duration</t>
-  </si>
-  <si>
-    <t>Max Throttle Value</t>
-  </si>
-  <si>
-    <t>Max Steering Angle</t>
-  </si>
-  <si>
-    <t>Max Steering Angle Rate</t>
-  </si>
-  <si>
-    <t>Max Yaw Rate</t>
-  </si>
-  <si>
-    <t>Max Lateral Acceleration</t>
-  </si>
-  <si>
-    <t>synonym</t>
-  </si>
-  <si>
-    <t>genericName</t>
-  </si>
-  <si>
-    <t>raster</t>
-  </si>
-  <si>
-    <t>latActAccel</t>
-  </si>
-  <si>
-    <t>longActAccel</t>
-  </si>
-  <si>
-    <t>aebTargetDecel</t>
-  </si>
-  <si>
-    <t>speedESC</t>
-  </si>
-  <si>
-    <t>egoSpeed</t>
-  </si>
-  <si>
-    <t>throttleValue</t>
-  </si>
-  <si>
-    <t>aebAbortFromVcs</t>
-  </si>
-  <si>
-    <t>brakePedalPressed</t>
-  </si>
-  <si>
-    <t>steerWheelAngle</t>
-  </si>
-  <si>
-    <t>steerWheelAngleSpeed</t>
-  </si>
-  <si>
-    <t>yawRate</t>
-  </si>
-  <si>
-    <t>aeb_state_info/most_relevant_object_id</t>
-  </si>
-  <si>
-    <t>targetId</t>
-  </si>
-  <si>
-    <t>aeb_state_info/time_to_collision</t>
-  </si>
-  <si>
-    <t>ttc</t>
-  </si>
-  <si>
-    <t>aeb_state_info/aeb_full_state_info/state</t>
-  </si>
-  <si>
-    <t>aebFullState</t>
-  </si>
-  <si>
-    <t>aeb_state_info/aeb_partial_state_info/state</t>
-  </si>
-  <si>
-    <t>aebPartialState</t>
-  </si>
-  <si>
-    <t>plotEnabled</t>
-  </si>
-  <si>
-    <t>Ego Speed (km/h)</t>
-  </si>
-  <si>
-    <t>Time (sec)</t>
-  </si>
-  <si>
-    <t>Percentage (%)</t>
-  </si>
-  <si>
-    <t>Angle (rad)</t>
-  </si>
-  <si>
-    <t>Angle Speed (rad/s)</t>
-  </si>
-  <si>
-    <t>Acceleration (m/s2)</t>
-  </si>
-  <si>
-    <t>Distance (m)</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Stable Detection Dist</t>
-  </si>
-  <si>
-    <t>AEB Actuation Dist</t>
-  </si>
-  <si>
-    <t>AEB Stop Gap</t>
-  </si>
-  <si>
-    <t>stableDetDist</t>
-  </si>
-  <si>
-    <t>aebIntvDist</t>
-  </si>
-  <si>
-    <t>aebStopGap</t>
-  </si>
-  <si>
-    <t>AEB Braking Distances</t>
-  </si>
-  <si>
-    <t>ConnectPoints</t>
-  </si>
-  <si>
-    <t>firstDetDist</t>
-  </si>
-  <si>
-    <t>First Detection Dist</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>^</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Shapes</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>vehicleIOActuationFeedback</t>
+    <t>AEB Intervention Duration</t>
+  </si>
+  <si>
+    <t>Vehicle Response Dead Time</t>
+  </si>
+  <si>
+    <t>Max Yaw Rate Before AEB</t>
+  </si>
+  <si>
+    <t>Max Lateral Acceleration Before AEB</t>
   </si>
 </sst>
 </file>
@@ -768,7 +780,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -780,24 +792,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -805,10 +817,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -816,142 +828,142 @@
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="C16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1056,12 +1068,12 @@
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
@@ -1074,42 +1086,42 @@
   <sheetData>
     <row r="2" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -1118,19 +1130,19 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="2" t="b">
         <v>0</v>
@@ -1138,10 +1150,10 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1150,19 +1162,19 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="2" t="b">
         <v>0</v>
@@ -1170,10 +1182,10 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1182,19 +1194,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="2" t="b">
         <v>0</v>
@@ -1202,10 +1214,10 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1214,19 +1226,19 @@
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="2" t="b">
         <v>0</v>
@@ -1234,10 +1246,10 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1246,19 +1258,19 @@
         <v>300</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="2" t="b">
         <v>0</v>
@@ -1266,10 +1278,10 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1278,19 +1290,19 @@
         <v>600</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" s="2" t="b">
         <v>0</v>
@@ -1298,10 +1310,10 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1310,19 +1322,19 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="2" t="b">
         <v>0</v>
@@ -1330,10 +1342,10 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1342,19 +1354,19 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="2" t="b">
         <v>0</v>
@@ -1362,10 +1374,10 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1374,19 +1386,19 @@
         <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="2" t="b">
         <v>1</v>
@@ -1394,10 +1406,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1406,19 +1418,19 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="2" t="b">
         <v>1</v>
@@ -1426,10 +1438,10 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1438,19 +1450,19 @@
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="2" t="b">
         <v>1</v>
@@ -1458,10 +1470,10 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1470,19 +1482,19 @@
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" s="2" t="b">
         <v>1</v>
@@ -1505,47 +1517,47 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1565,13 +1577,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>